<commit_message>
auto:removing first name,last name and date of birth from the call form
</commit_message>
<xml_diff>
--- a/config/forms/app/call.xlsx
+++ b/config/forms/app/call.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="100">
   <si>
     <t>type</t>
   </si>
@@ -72,6 +72,18 @@
     <t>source_id</t>
   </si>
   <si>
+    <t>my_field_fst</t>
+  </si>
+  <si>
+    <t>my_field_lst</t>
+  </si>
+  <si>
+    <t>my_field_dob</t>
+  </si>
+  <si>
+    <t>my_field_address</t>
+  </si>
+  <si>
     <t>contact</t>
   </si>
   <si>
@@ -129,22 +141,7 @@
     <t>call</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>birth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of Birth </t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>Current Address</t>
   </si>
   <si>
     <t>call1</t>
@@ -411,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -435,6 +432,12 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -697,6 +700,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.13"/>
+    <col customWidth="1" min="2" max="2" width="18.13"/>
     <col customWidth="1" min="3" max="3" width="66.38"/>
     <col customWidth="1" min="4" max="4" width="33.75"/>
   </cols>
@@ -811,14 +815,12 @@
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -831,19 +833,15 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="C6" s="7"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -854,19 +852,15 @@
       <c r="M6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="A7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="7"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -877,19 +871,15 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -900,19 +890,17 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
+      <c r="A9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -927,14 +915,14 @@
         <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -946,17 +934,19 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>28</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -967,17 +957,19 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>19</v>
+      <c r="A12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -989,10 +981,10 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>13</v>
@@ -1012,10 +1004,10 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>13</v>
@@ -1034,11 +1026,15 @@
       <c r="M14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
+      <c r="A15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1051,11 +1047,15 @@
       <c r="M15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1068,13 +1068,19 @@
       <c r="M16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1085,15 +1091,21 @@
       <c r="M17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="F18" s="2"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1102,21 +1114,15 @@
       <c r="M18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="A19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1125,21 +1131,15 @@
       <c r="M19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1149,18 +1149,12 @@
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1171,19 +1165,15 @@
       <c r="M21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="A22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1192,19 +1182,21 @@
       <c r="M22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="10"/>
+      <c r="A23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1213,19 +1205,21 @@
       <c r="M23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>43</v>
+      <c r="A24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1234,17 +1228,19 @@
       <c r="M24" s="2"/>
     </row>
     <row r="25">
-      <c r="A25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>45</v>
+      <c r="A25" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1256,13 +1252,13 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1277,13 +1273,13 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1297,14 +1293,14 @@
       <c r="M27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="s">
-        <v>46</v>
+      <c r="A28" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1318,18 +1314,16 @@
       <c r="M28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="5" t="s">
-        <v>46</v>
+      <c r="A29" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1342,16 +1336,16 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1364,72 +1358,95 @@
       <c r="M30" s="2"/>
     </row>
     <row r="31">
-      <c r="A31" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="13" t="s">
+      <c r="A31" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+    </row>
+    <row r="33">
+      <c r="A33" s="15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="13" t="s">
+      <c r="B33" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="D33" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="13" t="s">
+    </row>
+    <row r="34">
+      <c r="A34" s="15" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="13" t="s">
+      <c r="B34" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="C34" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="D34" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="K34" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="K33" s="13" t="s">
+    </row>
+    <row r="35">
+      <c r="A35" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="13" t="s">
+      <c r="C35" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="13" t="s">
+    </row>
+    <row r="36">
+      <c r="A36" s="15" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="13" t="s">
+      <c r="B36" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="C36" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="13" t="s">
-        <v>30</v>
+    </row>
+    <row r="37">
+      <c r="A37" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1453,7 +1470,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1487,68 +1504,68 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="15" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+      <c r="B4" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="13" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="13" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="13" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="15" t="s">
         <v>88</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1570,49 +1587,49 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="17" t="s">
+      <c r="B2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="20" t="str">
+        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
+        <v>2022-10-24_12-52</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="18" t="str">
-        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-08-02_22-56</v>
-      </c>
-      <c r="D2" s="19" t="s">
+      <c r="E2" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="21" t="s">
         <v>99</v>
-      </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19" t="s">
-        <v>100</v>
       </c>
       <c r="H2" s="2"/>
     </row>

</xml_diff>

<commit_message>
auto:renaming call start a call log and start a routine visit forms
</commit_message>
<xml_diff>
--- a/config/forms/app/call.xlsx
+++ b/config/forms/app/call.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="110">
   <si>
     <t>type</t>
   </si>
@@ -138,9 +138,42 @@
     <t>../inputs/contact/name</t>
   </si>
   <si>
+    <t>fast_name_ctx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(instance('contact-summary')/context/fstname != '', instance('contact-summary')/context/fstname, .)        </t>
+  </si>
+  <si>
     <t>call</t>
   </si>
   <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>First name: ${fast_name_ctx}</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Current address</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
@@ -193,9 +226,6 @@
   </si>
   <si>
     <t>Was the patient’s identity verified?</t>
-  </si>
-  <si>
-    <t>note</t>
   </si>
   <si>
     <t>note_verified</t>
@@ -306,7 +336,7 @@
     <t>default_language</t>
   </si>
   <si>
-    <t xml:space="preserve">Start Call Log
+    <t xml:space="preserve"> Call Log
 </t>
   </si>
   <si>
@@ -408,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -444,6 +474,15 @@
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -703,6 +742,7 @@
     <col customWidth="1" min="2" max="2" width="18.13"/>
     <col customWidth="1" min="3" max="3" width="66.38"/>
     <col customWidth="1" min="4" max="4" width="33.75"/>
+    <col customWidth="1" min="7" max="7" width="88.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1229,20 +1269,20 @@
     </row>
     <row r="25">
       <c r="A25" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="14" t="s">
+        <v>42</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1251,17 +1291,19 @@
       <c r="M25" s="2"/>
     </row>
     <row r="26">
-      <c r="A26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>44</v>
+      <c r="C26" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1272,14 +1314,14 @@
       <c r="M26" s="2"/>
     </row>
     <row r="27">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1293,14 +1335,14 @@
       <c r="M27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1314,14 +1356,14 @@
       <c r="M28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1335,18 +1377,16 @@
       <c r="M29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1359,17 +1399,15 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1381,71 +1419,180 @@
       <c r="M31" s="2"/>
     </row>
     <row r="32">
-      <c r="A32" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="15" t="s">
+      <c r="A32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="15" t="s">
+      <c r="C33" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C34" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="15" t="s">
+      <c r="C35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="D35" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="C36" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K34" s="15" t="s">
+      <c r="D36" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="15" t="s">
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K39" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="15" t="s">
+      <c r="B40" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="18" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1470,7 +1617,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1504,68 +1651,68 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>82</v>
+      <c r="A4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>84</v>
+      <c r="A5" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>86</v>
+      <c r="A6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>88</v>
+      <c r="A7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1587,49 +1734,49 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>95</v>
+      <c r="A1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="20" t="str">
+      <c r="A2" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="23" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-10-24_12-52</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21" t="s">
-        <v>99</v>
+        <v>2022-11-03_09-24</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
+        <v>109</v>
       </c>
       <c r="H2" s="2"/>
     </row>

</xml_diff>

<commit_message>
auto:adding tsis number,aka to the context object plus message from Textit triggers this outbound configuration
</commit_message>
<xml_diff>
--- a/config/forms/app/call.xlsx
+++ b/config/forms/app/call.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="130">
   <si>
     <t>type</t>
   </si>
@@ -72,6 +72,9 @@
     <t>my_field_address</t>
   </si>
   <si>
+    <t>my_field_tsis</t>
+  </si>
+  <si>
     <t>contact</t>
   </si>
   <si>
@@ -105,6 +108,12 @@
     <t>address</t>
   </si>
   <si>
+    <t>aka</t>
+  </si>
+  <si>
+    <t>tsis</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
@@ -144,6 +153,18 @@
     <t>../inputs/contact/address</t>
   </si>
   <si>
+    <t>patient_aka</t>
+  </si>
+  <si>
+    <t>../inputs/contact/aka</t>
+  </si>
+  <si>
+    <t>patient_tsis</t>
+  </si>
+  <si>
+    <t>../inputs/contact/tsis</t>
+  </si>
+  <si>
     <t>patient_date_of_birth</t>
   </si>
   <si>
@@ -177,6 +198,18 @@
     <t>if(instance('contact-summary')/context/address != '', instance('contact-summary')/context/address, .)</t>
   </si>
   <si>
+    <t>aka_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_aka != '', instance('contact-summary')/context/patient_aka, .)</t>
+  </si>
+  <si>
+    <t>tsis_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_tsis != '', instance('contact-summary')/context/patient_tsis, .)</t>
+  </si>
+  <si>
     <t>call</t>
   </si>
   <si>
@@ -186,19 +219,19 @@
     <t>first_name</t>
   </si>
   <si>
-    <t>**First name:** ${fast_name_ctx}</t>
+    <t xml:space="preserve"> ${fast_name_ctx}  ${last_name_ctx}</t>
   </si>
   <si>
     <t>last_name</t>
   </si>
   <si>
-    <t>**Last name:** ${last_name_ctx}</t>
+    <t>${aka_ctx}  |   ${date_of_birth_ctx}</t>
   </si>
   <si>
     <t>dob</t>
   </si>
   <si>
-    <t>**Date of birth:**   ${date_of_birth_ctx}</t>
+    <t>${tsis_ctx}</t>
   </si>
   <si>
     <t>**Current address:**  ${address_ctx}</t>
@@ -225,7 +258,7 @@
     <t>verify_date</t>
   </si>
   <si>
-    <t>Did the patient verify the correct date of birth?</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>match</t>
@@ -810,49 +843,43 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
@@ -863,10 +890,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
@@ -877,7 +904,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>27</v>
@@ -891,7 +918,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>28</v>
@@ -905,7 +932,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>29</v>
@@ -919,7 +946,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>30</v>
@@ -927,24 +954,30 @@
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
@@ -955,259 +988,280 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>61</v>
+        <v>9</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>62</v>
+        <v>9</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>65</v>
+        <v>9</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>70</v>
+        <v>9</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="42">
@@ -1215,10 +1269,10 @@
         <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43">
@@ -1226,13 +1280,10 @@
         <v>66</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44">
@@ -1240,13 +1291,10 @@
         <v>66</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45">
@@ -1254,65 +1302,148 @@
         <v>66</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>32</v>
+        <v>77</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1467,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1347,68 +1478,68 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1428,48 +1559,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="H1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-11-09_23-20</v>
+        <v>2023-06-09_16-52</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="H2" s="5"/>
     </row>

</xml_diff>

<commit_message>
auto:change context for call form and adding patient identity card on top
</commit_message>
<xml_diff>
--- a/config/forms/app/call.xlsx
+++ b/config/forms/app/call.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="136">
   <si>
     <t>type</t>
   </si>
@@ -114,6 +114,9 @@
     <t>tsis</t>
   </si>
   <si>
+    <t>at</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
@@ -165,6 +168,12 @@
     <t>../inputs/contact/tsis</t>
   </si>
   <si>
+    <t>patient_at</t>
+  </si>
+  <si>
+    <t>../inputs/contact/at</t>
+  </si>
+  <si>
     <t>patient_date_of_birth</t>
   </si>
   <si>
@@ -210,6 +219,19 @@
     <t>if(instance('contact-summary')/context/patient_tsis != '', instance('contact-summary')/context/patient_tsis, .)</t>
   </si>
   <si>
+    <t>at_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_at != '', instance('contact-summary')/context/patient_at, .)</t>
+  </si>
+  <si>
+    <t>yr_date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int(int(format-date(today(), "%Y") - format-date(${date_of_birth_ctx}, "%Y")) )
+</t>
+  </si>
+  <si>
     <t>call</t>
   </si>
   <si>
@@ -219,13 +241,16 @@
     <t>first_name</t>
   </si>
   <si>
-    <t xml:space="preserve"> ${fast_name_ctx}  ${last_name_ctx}</t>
+    <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}  ${last_name_ctx}**&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1 yellow </t>
   </si>
   <si>
     <t>last_name</t>
   </si>
   <si>
-    <t>${aka_ctx}  |   ${date_of_birth_ctx}</t>
+    <t>${aka_ctx}  |  ${yr_date_of_birth_ctx} yr   ${at_ctx}</t>
   </si>
   <si>
     <t>dob</t>
@@ -253,12 +278,6 @@
   </si>
   <si>
     <t>Did the patient verify the correct last name?</t>
-  </si>
-  <si>
-    <t>verify_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>match</t>
@@ -736,7 +755,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="23.0"/>
     <col customWidth="1" min="2" max="2" width="31.13"/>
-    <col customWidth="1" min="3" max="3" width="59.38"/>
+    <col customWidth="1" min="3" max="3" width="67.5"/>
     <col customWidth="1" min="4" max="4" width="41.88"/>
     <col customWidth="1" min="7" max="7" width="79.38"/>
   </cols>
@@ -988,13 +1007,16 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -1002,7 +1024,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
@@ -1010,16 +1032,13 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="23">
@@ -1027,7 +1046,7 @@
         <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>9</v>
@@ -1038,34 +1057,40 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28">
@@ -1073,377 +1098,419 @@
         <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>73</v>
+        <v>9</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>35</v>
+        <v>101</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1467,7 +1534,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1478,68 +1545,68 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1559,48 +1626,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="H1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-06-09_16-52</v>
+        <v>2023-06-16_16-44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H2" s="5"/>
     </row>

</xml_diff>

<commit_message>
auto:changing the call and create forms for reflect data from the enrollment form
</commit_message>
<xml_diff>
--- a/config/forms/app/call.xlsx
+++ b/config/forms/app/call.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="130">
   <si>
     <t>type</t>
   </si>
@@ -105,9 +105,6 @@
     <t>name1</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>aka</t>
   </si>
   <si>
@@ -150,12 +147,6 @@
     <t>../inputs/contact/name1</t>
   </si>
   <si>
-    <t>patient_address</t>
-  </si>
-  <si>
-    <t>../inputs/contact/address</t>
-  </si>
-  <si>
     <t>patient_aka</t>
   </si>
   <si>
@@ -199,12 +190,6 @@
   </si>
   <si>
     <t>if(instance('contact-summary')/context/patient_date_of_birth != '', instance('contact-summary')/context/patient_date_of_birth, .)</t>
-  </si>
-  <si>
-    <t>address_ctx</t>
-  </si>
-  <si>
-    <t>if(instance('contact-summary')/context/address != '', instance('contact-summary')/context/address, .)</t>
   </si>
   <si>
     <t>aka_ctx</t>
@@ -257,9 +242,6 @@
   </si>
   <si>
     <t>${tsis_ctx}</t>
-  </si>
-  <si>
-    <t>**Current address:**  ${address_ctx}</t>
   </si>
   <si>
     <t>date</t>
@@ -1007,16 +989,13 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -1024,7 +1003,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
@@ -1032,13 +1011,16 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="23">
@@ -1046,7 +1028,7 @@
         <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>9</v>
@@ -1057,40 +1039,34 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -1098,419 +1074,372 @@
         <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>67</v>
+      <c r="E42" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1463,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1545,68 +1474,68 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1626,48 +1555,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="H1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-06-16_16-44</v>
+        <v>2023-06-21_21-02</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H2" s="5"/>
     </row>

</xml_diff>

<commit_message>
auto:changes in the call log form
</commit_message>
<xml_diff>
--- a/config/forms/app/call.xlsx
+++ b/config/forms/app/call.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="125">
   <si>
     <t>type</t>
   </si>
@@ -102,6 +102,9 @@
     <t>sex</t>
   </si>
   <si>
+    <t>curr_address</t>
+  </si>
+  <si>
     <t>name1</t>
   </si>
   <si>
@@ -151,6 +154,12 @@
   </si>
   <si>
     <t>../inputs/contact/aka</t>
+  </si>
+  <si>
+    <t>cur_address</t>
+  </si>
+  <si>
+    <t>../inputs/contact/curr_address</t>
   </si>
   <si>
     <t>patient_tsis</t>
@@ -235,13 +244,30 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>${aka_ctx}  |  ${yr_date_of_birth_ctx} yr   ${at_ctx}</t>
+    <t>${aka_ctx}  |  ${yr_date_of_birth_ctx} yr   ${at_ctx}&lt;I class="fa fa-user"&gt;&lt;/i&gt;</t>
   </si>
   <si>
     <t>dob</t>
   </si>
   <si>
-    <t>${tsis_ctx}</t>
+    <t>${tsis_ctx}&lt;I class="fa fa-user"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>currnt_address</t>
+  </si>
+  <si>
+    <t>${cur_address}</t>
+  </si>
+  <si>
+    <t>note_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the Client’s identity:
+    1. Can you please remind me of your last name?
+    2. Please tell me your DOB? 
+    3. What is your current address?
+    4. What clinic did you last visit?
+</t>
   </si>
   <si>
     <t>date</t>
@@ -256,36 +282,6 @@
     <t>select_one yes_no</t>
   </si>
   <si>
-    <t>verify</t>
-  </si>
-  <si>
-    <t>Did the patient verify the correct last name?</t>
-  </si>
-  <si>
-    <t>match</t>
-  </si>
-  <si>
-    <t>Did the current address shared by the patient match the address in the system?</t>
-  </si>
-  <si>
-    <t>if_no</t>
-  </si>
-  <si>
-    <t>What was your previous address? Did the patient correctly verify previous address?</t>
-  </si>
-  <si>
-    <t>${match} = 'no'</t>
-  </si>
-  <si>
-    <t>if_yes</t>
-  </si>
-  <si>
-    <t>Did the patient move and do we need to update the address?</t>
-  </si>
-  <si>
-    <t>${match} = 'yes'</t>
-  </si>
-  <si>
     <t>identity</t>
   </si>
   <si>
@@ -295,7 +291,7 @@
     <t>note_verified</t>
   </si>
   <si>
-    <t>Patient was not verified, please end the call.</t>
+    <t>Patient was not verified, STOP please end the call.</t>
   </si>
   <si>
     <t>${identity} = 'no'</t>
@@ -353,12 +349,6 @@
   </si>
   <si>
     <t>Appointment confirmation</t>
-  </si>
-  <si>
-    <t>added_lab_appointment</t>
-  </si>
-  <si>
-    <t>Added Lab appointment</t>
   </si>
   <si>
     <t>answered_questions_about_care</t>
@@ -989,13 +979,16 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -1003,7 +996,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
@@ -1011,16 +1004,13 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="23">
@@ -1028,7 +1018,7 @@
         <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>9</v>
@@ -1039,34 +1029,40 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28">
@@ -1074,345 +1070,339 @@
         <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>73</v>
+        <v>9</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="C48" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="54">
@@ -1420,26 +1410,26 @@
         <v>25</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1463,7 +1453,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1474,68 +1464,57 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1555,48 +1534,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="H1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-06-21_21-02</v>
+        <v>2023-07-31_10-51</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H2" s="5"/>
     </row>

</xml_diff>

<commit_message>
auto:updating the patient identifier card on the call log form
</commit_message>
<xml_diff>
--- a/config/forms/app/call.xlsx
+++ b/config/forms/app/call.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="132">
   <si>
     <t>type</t>
   </si>
@@ -117,6 +117,9 @@
     <t>at</t>
   </si>
   <si>
+    <t>genda</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
@@ -172,6 +175,12 @@
   </si>
   <si>
     <t>../inputs/contact/at</t>
+  </si>
+  <si>
+    <t>patient_genda</t>
+  </si>
+  <si>
+    <t>../inputs/contact/genda</t>
   </si>
   <si>
     <t>patient_date_of_birth</t>
@@ -226,6 +235,12 @@
 </t>
   </si>
   <si>
+    <t>gender_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_genda != '', instance('contact-summary')/context/patient_genda, .)</t>
+  </si>
+  <si>
     <t>call</t>
   </si>
   <si>
@@ -241,28 +256,34 @@
     <t xml:space="preserve">h1 yellow </t>
   </si>
   <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>${aka_ctx}  |  ${yr_date_of_birth_ctx} yr   ${at_ctx}&lt;I class="fa fa-user"&gt;&lt;/i&gt;</t>
+    <t>nick</t>
+  </si>
+  <si>
+    <t>Nickname: **${aka_ctx}**</t>
+  </si>
+  <si>
+    <t>age_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age: **${yr_date_of_birth_ctx} yr**  </t>
+  </si>
+  <si>
+    <t>gender_n</t>
+  </si>
+  <si>
+    <t>Gender Identity: **${gender_ctx}**</t>
   </si>
   <si>
     <t>dob</t>
   </si>
   <si>
-    <t>${tsis_ctx}&lt;I class="fa fa-user"&gt;&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>currnt_address</t>
-  </si>
-  <si>
-    <t>${cur_address}</t>
+    <t>TSIS: **${tsis_ctx}**</t>
   </si>
   <si>
     <t>note_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify the Client’s identity:
+    <t xml:space="preserve">**Verify the Client’s identity:**
     1. Can you please remind me of your last name?
     2. Please tell me your DOB? 
     3. What is your current address?
@@ -401,7 +422,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -412,6 +433,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -429,12 +454,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -476,29 +507,32 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -993,7 +1027,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>34</v>
@@ -1001,13 +1035,14 @@
       <c r="C21" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>9</v>
@@ -1015,16 +1050,13 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="24">
@@ -1032,7 +1064,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>9</v>
@@ -1043,34 +1075,40 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29">
@@ -1078,358 +1116,408 @@
         <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>76</v>
+        <v>9</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>78</v>
+        <v>9</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="E49" s="1"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="E50" s="1"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>88</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E51" s="1"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>36</v>
+        <v>76</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1453,7 +1541,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1464,57 +1552,57 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1533,51 +1621,51 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="5"/>
+      <c r="A1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="6"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="7" t="str">
+      <c r="A2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="8" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-07-31_10-51</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" s="5"/>
+        <v>2023-07-31_17-02</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
auto:formatting changes and removing some reports
</commit_message>
<xml_diff>
--- a/config/forms/app/call.xlsx
+++ b/config/forms/app/call.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="134">
   <si>
     <t>type</t>
   </si>
@@ -244,16 +244,16 @@
     <t>call</t>
   </si>
   <si>
+    <t>field-list summary</t>
+  </si>
+  <si>
     <t>note</t>
   </si>
   <si>
     <t>first_name</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}  ${last_name_ctx}**&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h1 yellow </t>
+    <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}**&lt;/i&gt;</t>
   </si>
   <si>
     <t>nick</t>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>TSIS: **${tsis_ctx}**</t>
+  </si>
+  <si>
+    <t>n_special_instruction_title</t>
+  </si>
+  <si>
+    <t>h1 yellow</t>
   </si>
   <si>
     <t>note_1</t>
@@ -422,7 +428,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -439,14 +445,24 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="8.0"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -454,7 +470,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +481,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
+        <bgColor rgb="FFFCE5CD"/>
       </patternFill>
     </fill>
   </fills>
@@ -507,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -517,22 +539,37 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1368,26 +1405,24 @@
         <v>9</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E48" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="E48" s="1"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>80</v>
@@ -1399,7 +1434,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>82</v>
@@ -1411,7 +1446,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>84</v>
@@ -1423,7 +1458,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>86</v>
@@ -1433,41 +1468,67 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B53" s="1" t="s">
+      <c r="A53" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7" t="s">
         <v>89</v>
       </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="6"/>
+      <c r="T53" s="6"/>
+      <c r="U53" s="6"/>
+      <c r="V53" s="6"/>
+      <c r="W53" s="6"/>
+      <c r="X53" s="6"/>
+      <c r="Y53" s="6"/>
+      <c r="Z53" s="6"/>
+      <c r="AA53" s="6"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>96</v>
@@ -1475,52 +1536,68 @@
       <c r="C56" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="D53">
+      <formula1>"yes,no"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1541,7 +1618,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1552,57 +1629,57 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1621,51 +1698,51 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="6"/>
+      <c r="F1" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H1" s="11"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="8" t="str">
+      <c r="C2" s="13" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-07-31_17-02</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+        <v>2023-08-03_20-19</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="E2" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="11"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
auto:adding more fields in the call log form
</commit_message>
<xml_diff>
--- a/config/forms/app/call.xlsx
+++ b/config/forms/app/call.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="148">
   <si>
     <t>type</t>
   </si>
@@ -120,12 +120,15 @@
     <t>genda</t>
   </si>
   <si>
+    <t>docket</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
-    <t>phone</t>
-  </si>
-  <si>
     <t>end group</t>
   </si>
   <si>
@@ -169,6 +172,18 @@
   </si>
   <si>
     <t>../inputs/contact/tsis</t>
+  </si>
+  <si>
+    <t>patient_phone</t>
+  </si>
+  <si>
+    <t>../inputs/contact/phone</t>
+  </si>
+  <si>
+    <t>patient_docket</t>
+  </si>
+  <si>
+    <t>../inputs/contact/docket</t>
   </si>
   <si>
     <t>patient_at</t>
@@ -241,6 +256,24 @@
     <t>if(instance('contact-summary')/context/patient_genda != '', instance('contact-summary')/context/patient_genda, .)</t>
   </si>
   <si>
+    <t>address_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/cur_address != '', instance('contact-summary')/context/cur_address, .)</t>
+  </si>
+  <si>
+    <t>docket_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_docket != '', instance('contact-summary')/context/patient_docket, .)</t>
+  </si>
+  <si>
+    <t>phone_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_phone != '', instance('contact-summary')/context/patient_phone, .)</t>
+  </si>
+  <si>
     <t>call</t>
   </si>
   <si>
@@ -256,16 +289,37 @@
     <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}**&lt;/i&gt;</t>
   </si>
   <si>
+    <t>birth_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Birth: **${date_of_birth_ctx}**  </t>
+  </si>
+  <si>
     <t>age_n</t>
   </si>
   <si>
-    <t xml:space="preserve">Age: **${yr_date_of_birth_ctx} yr**  </t>
+    <t xml:space="preserve">Current Age: **${yr_date_of_birth_ctx} yr**  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Docket Number: **${docket_ctx}**  </t>
   </si>
   <si>
     <t>dob</t>
   </si>
   <si>
     <t>TSIS: **${tsis_ctx}**</t>
+  </si>
+  <si>
+    <t>fon_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone Number:  **${phone_ctx}**  </t>
+  </si>
+  <si>
+    <t>current_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Address: **${address_ctx}**  </t>
   </si>
   <si>
     <t>n_special_instruction_title</t>
@@ -291,7 +345,7 @@
     <t>call1</t>
   </si>
   <si>
-    <t xml:space="preserve">Date of Call the call </t>
+    <t xml:space="preserve">Date of Call </t>
   </si>
   <si>
     <t>select_one yes_no</t>
@@ -1064,7 +1118,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>35</v>
@@ -1072,65 +1126,77 @@
       <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>20</v>
@@ -1138,10 +1204,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="30">
@@ -1149,13 +1215,7 @@
         <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31">
@@ -1163,402 +1223,540 @@
         <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>74</v>
+      <c r="G46" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>76</v>
+      <c r="G47" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E48" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E49" s="1"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>83</v>
+        <v>9</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-      <c r="Q51" s="6"/>
-      <c r="R51" s="6"/>
-      <c r="S51" s="6"/>
-      <c r="T51" s="6"/>
-      <c r="U51" s="6"/>
-      <c r="V51" s="6"/>
-      <c r="W51" s="6"/>
-      <c r="X51" s="6"/>
-      <c r="Y51" s="6"/>
-      <c r="Z51" s="6"/>
-      <c r="AA51" s="6"/>
+      <c r="A51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>90</v>
+        <v>9</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>93</v>
+        <v>9</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="E55" s="1"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>100</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E56" s="1"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>102</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E57" s="1"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="E58" s="1"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>37</v>
+        <v>88</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="6"/>
+      <c r="E62" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="6"/>
+      <c r="P62" s="6"/>
+      <c r="Q62" s="6"/>
+      <c r="R62" s="6"/>
+      <c r="S62" s="6"/>
+      <c r="T62" s="6"/>
+      <c r="U62" s="6"/>
+      <c r="V62" s="6"/>
+      <c r="W62" s="6"/>
+      <c r="X62" s="6"/>
+      <c r="Y62" s="6"/>
+      <c r="Z62" s="6"/>
+      <c r="AA62" s="6"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D51">
+    <dataValidation type="list" allowBlank="1" sqref="D62">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1582,7 +1780,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1593,57 +1791,57 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1663,48 +1861,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="H1" s="11"/>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C2" s="13" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-09-28_11-59</v>
+        <v>2024-04-16_16-39</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="H2" s="11"/>
     </row>

</xml_diff>

<commit_message>
updating reports for the call log form
</commit_message>
<xml_diff>
--- a/config/forms/app/call.xlsx
+++ b/config/forms/app/call.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="149">
   <si>
     <t>type</t>
   </si>
@@ -22,6 +22,9 @@
   </si>
   <si>
     <t>label</t>
+  </si>
+  <si>
+    <t>instance::tag</t>
   </si>
   <si>
     <t>relevant</t>
@@ -840,9 +843,10 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="23.0"/>
     <col customWidth="1" min="2" max="2" width="31.13"/>
-    <col customWidth="1" min="3" max="3" width="67.5"/>
-    <col customWidth="1" min="4" max="4" width="41.88"/>
-    <col customWidth="1" min="7" max="7" width="79.38"/>
+    <col customWidth="1" min="3" max="3" width="31.75"/>
+    <col customWidth="1" min="4" max="4" width="29.63"/>
+    <col customWidth="1" min="5" max="5" width="41.88"/>
+    <col customWidth="1" min="8" max="8" width="79.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -867,783 +871,893 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D24" s="1"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D25" s="1"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G32" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>46</v>
+        <v>10</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>48</v>
+        <v>10</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>52</v>
+        <v>10</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>54</v>
+        <v>10</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>56</v>
+        <v>10</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>58</v>
+        <v>10</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>60</v>
+        <v>10</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G42" s="1" t="s">
         <v>63</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>65</v>
+        <v>10</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>67</v>
+        <v>10</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>69</v>
+        <v>10</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>71</v>
+        <v>10</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>73</v>
+        <v>10</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>75</v>
+        <v>10</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>77</v>
+        <v>10</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>81</v>
+        <v>10</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>83</v>
+        <v>10</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>85</v>
+        <v>10</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>87</v>
+        <v>10</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="F54" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E55" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="1"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E56" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="1"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E57" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="1"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E58" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="1"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F62" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="6"/>
+      <c r="F62" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
@@ -1665,98 +1779,110 @@
       <c r="Y62" s="6"/>
       <c r="Z62" s="6"/>
       <c r="AA62" s="6"/>
+      <c r="AB62" s="6"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>108</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D64" s="1"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>111</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="D65" s="1"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>114</v>
+        <v>13</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D67" s="1" t="s">
         <v>118</v>
+      </c>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>120</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="D68" s="1"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>123</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D69" s="1"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D62">
+    <dataValidation type="list" allowBlank="1" sqref="E62">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1780,7 +1906,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1791,57 +1917,57 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1861,48 +1987,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H1" s="11"/>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" s="13" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2024-04-16_16-39</v>
+        <v>2024-07-08_22-28</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H2" s="11"/>
     </row>

</xml_diff>